<commit_message>
Finished wrangle first pass
</commit_message>
<xml_diff>
--- a/0_data/Empty slots.xlsx
+++ b/0_data/Empty slots.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11211"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jamescookuniversity-my.sharepoint.com/personal/benjamin_cresswell_jcu_edu_au/Documents/Ben PhD/Data &amp; analysis/Keppels/Subsampling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jamescookuniversity-my.sharepoint.com/personal/benjamin_cresswell_jcu_edu_au/Documents/Ben PhD/Data &amp; analysis/Keppels/Keppels_subsampling/0_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_29EC5492B49F687942C1C6CC6C5DABBF99C4D3AC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2888CD7-F30F-854B-9186-08ABEE142F6F}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_29EC5492B49F687942C1C6CC6C5DABBF99C4D3AC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{150073AE-86E6-D344-8A08-4AB946401325}"/>
   <bookViews>
     <workbookView xWindow="15140" yWindow="760" windowWidth="15100" windowHeight="18880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,141 +42,21 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>PMJuv01</t>
-  </si>
-  <si>
-    <t>B1</t>
-  </si>
-  <si>
     <t>Fin</t>
   </si>
   <si>
-    <t>PMJuv02</t>
-  </si>
-  <si>
-    <t>B2</t>
-  </si>
-  <si>
-    <t>PMJuv03</t>
-  </si>
-  <si>
-    <t>B3</t>
-  </si>
-  <si>
-    <t>PMJuv04</t>
-  </si>
-  <si>
-    <t>B4</t>
-  </si>
-  <si>
-    <t>PMJuv05</t>
-  </si>
-  <si>
-    <t>B5</t>
-  </si>
-  <si>
-    <t>PMJuv06</t>
-  </si>
-  <si>
-    <t>B6</t>
-  </si>
-  <si>
-    <t>PMJuv07</t>
-  </si>
-  <si>
-    <t>B7</t>
-  </si>
-  <si>
-    <t>PMJuv08</t>
-  </si>
-  <si>
-    <t>B8</t>
-  </si>
-  <si>
-    <t>PMAd01</t>
-  </si>
-  <si>
-    <t>E1</t>
-  </si>
-  <si>
-    <t>PMAd02</t>
-  </si>
-  <si>
-    <t>E2</t>
-  </si>
-  <si>
     <t>Tissue</t>
   </si>
   <si>
-    <t>PMAd03</t>
-  </si>
-  <si>
-    <t>E3</t>
-  </si>
-  <si>
-    <t>PMAd04</t>
-  </si>
-  <si>
-    <t>E4</t>
-  </si>
-  <si>
-    <t>PMAd05</t>
-  </si>
-  <si>
-    <t>E5</t>
-  </si>
-  <si>
-    <t>PMAd06</t>
-  </si>
-  <si>
-    <t>E6</t>
-  </si>
-  <si>
-    <t>PMAd07</t>
-  </si>
-  <si>
-    <t>E7</t>
-  </si>
-  <si>
-    <t>PMAd08</t>
-  </si>
-  <si>
-    <t>E8</t>
-  </si>
-  <si>
     <t>Scale</t>
   </si>
   <si>
-    <t>PMAd09</t>
-  </si>
-  <si>
-    <t>E9</t>
-  </si>
-  <si>
-    <t>PMAd10</t>
-  </si>
-  <si>
     <t>E10</t>
   </si>
   <si>
     <t>Only 7 samples</t>
   </si>
   <si>
-    <t>PMJuv09</t>
-  </si>
-  <si>
-    <t>PMJuv10</t>
-  </si>
-  <si>
-    <t>PMJuv11</t>
-  </si>
-  <si>
-    <t>PMJuv12</t>
-  </si>
-  <si>
-    <t>B9</t>
-  </si>
-  <si>
     <t>B10</t>
   </si>
   <si>
@@ -196,6 +76,126 @@
   </si>
   <si>
     <t>KI3.2 Box4</t>
+  </si>
+  <si>
+    <t>B01</t>
+  </si>
+  <si>
+    <t>B02</t>
+  </si>
+  <si>
+    <t>B03</t>
+  </si>
+  <si>
+    <t>B04</t>
+  </si>
+  <si>
+    <t>B05</t>
+  </si>
+  <si>
+    <t>B06</t>
+  </si>
+  <si>
+    <t>B07</t>
+  </si>
+  <si>
+    <t>B08</t>
+  </si>
+  <si>
+    <t>B09</t>
+  </si>
+  <si>
+    <t>E01</t>
+  </si>
+  <si>
+    <t>E02</t>
+  </si>
+  <si>
+    <t>E03</t>
+  </si>
+  <si>
+    <t>E04</t>
+  </si>
+  <si>
+    <t>E05</t>
+  </si>
+  <si>
+    <t>E06</t>
+  </si>
+  <si>
+    <t>E07</t>
+  </si>
+  <si>
+    <t>E08</t>
+  </si>
+  <si>
+    <t>E09</t>
+  </si>
+  <si>
+    <t>PMJuv21_01</t>
+  </si>
+  <si>
+    <t>PMJuv21_02</t>
+  </si>
+  <si>
+    <t>PMJuv21_03</t>
+  </si>
+  <si>
+    <t>PMJuv21_04</t>
+  </si>
+  <si>
+    <t>PMJuv21_05</t>
+  </si>
+  <si>
+    <t>PMJuv21_06</t>
+  </si>
+  <si>
+    <t>PMJuv21_07</t>
+  </si>
+  <si>
+    <t>PMJuv21_08</t>
+  </si>
+  <si>
+    <t>PMJuv21_09</t>
+  </si>
+  <si>
+    <t>PMJuv21_10</t>
+  </si>
+  <si>
+    <t>PMJuv21_11</t>
+  </si>
+  <si>
+    <t>PMJuv21_12</t>
+  </si>
+  <si>
+    <t>PMAd21_01</t>
+  </si>
+  <si>
+    <t>PMAd21_02</t>
+  </si>
+  <si>
+    <t>PMAd21_03</t>
+  </si>
+  <si>
+    <t>PMAd21_04</t>
+  </si>
+  <si>
+    <t>PMAd21_05</t>
+  </si>
+  <si>
+    <t>PMAd21_06</t>
+  </si>
+  <si>
+    <t>PMAd21_07</t>
+  </si>
+  <si>
+    <t>PMAd21_08</t>
+  </si>
+  <si>
+    <t>PMAd21_09</t>
+  </si>
+  <si>
+    <t>PMAd21_10</t>
   </si>
 </sst>
 </file>
@@ -272,6 +272,14 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -596,13 +604,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -634,259 +645,259 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" t="s">
-        <v>56</v>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C28" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" t="s">
-        <v>44</v>
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>